<commit_message>
write characteristics, first draft
</commit_message>
<xml_diff>
--- a/geo-plugin-manager/fileName.xlsx
+++ b/geo-plugin-manager/fileName.xlsx
@@ -2012,7 +2012,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="200">
   <si>
     <t># This section describes the overall experiment.</t>
   </si>
@@ -2705,18 +2705,27 @@
     <t>this is a title</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>blabla</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>file3.fastq</t>
   </si>
   <si>
     <t>illumina</t>
   </si>
   <si>
+    <t>characteristics: treatment</t>
+  </si>
+  <si>
+    <t>characteristics: genotype</t>
+  </si>
+  <si>
+    <t>characteristics: other</t>
+  </si>
+  <si>
     <t>Human</t>
   </si>
   <si>
@@ -2724,6 +2733,21 @@
   </si>
   <si>
     <t>blablbl</t>
+  </si>
+  <si>
+    <t>sample 2</t>
+  </si>
+  <si>
+    <t>sample 3</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>mutant</t>
+  </si>
+  <si>
+    <t>wildtype</t>
   </si>
 </sst>
 </file>
@@ -3435,13 +3459,13 @@
         <v>8</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>34</v>
+        <v>189</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>34</v>
+        <v>190</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>9</v>
@@ -3458,35 +3482,50 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C22" t="s">
-        <v>189</v>
+        <v>192</v>
+      </c>
+      <c r="E22" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C23" t="s">
-        <v>189</v>
+        <v>192</v>
+      </c>
+      <c r="E23" t="s">
+        <v>197</v>
+      </c>
+      <c r="F23" t="s">
+        <v>199</v>
+      </c>
+      <c r="G23" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
@@ -3544,7 +3583,7 @@
         <v>15</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
@@ -3595,9 +3634,7 @@
       <c r="A41" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>185</v>
-      </c>
+      <c r="B41" s="9"/>
       <c r="C41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -3606,7 +3643,9 @@
       <c r="A42" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="9"/>
+      <c r="B42" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="C42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>

</xml_diff>

<commit_message>
store files correctly in sampleobject
</commit_message>
<xml_diff>
--- a/geo-plugin-manager/fileName.xlsx
+++ b/geo-plugin-manager/fileName.xlsx
@@ -656,7 +656,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C62" shapeId="0">
+    <comment authorId="0" ref="C68" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -670,7 +670,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D62" shapeId="0">
+    <comment authorId="0" ref="D68" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2012,7 +2012,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="208">
   <si>
     <t># This section describes the overall experiment.</t>
   </si>
@@ -2711,10 +2711,34 @@
     <t>blabla</t>
   </si>
   <si>
+    <t>file4.fastq</t>
+  </si>
+  <si>
+    <t>illumina</t>
+  </si>
+  <si>
+    <t>file5.fastq</t>
+  </si>
+  <si>
+    <t>file6.fastq</t>
+  </si>
+  <si>
+    <t>file1.fastq</t>
+  </si>
+  <si>
+    <t>file2.fastq</t>
+  </si>
+  <si>
     <t>file3.fastq</t>
   </si>
   <si>
-    <t>illumina</t>
+    <t>file1.fastq.gz</t>
+  </si>
+  <si>
+    <t>file2.fastq.gz</t>
+  </si>
+  <si>
+    <t>file3.fastq.gz</t>
   </si>
   <si>
     <t>characteristics: treatment</t>
@@ -3274,7 +3298,7 @@
   <sheetPr>
     <tabColor indexed="14"/>
   </sheetPr>
-  <dimension ref="A1:L228"/>
+  <dimension ref="A1:L234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -3459,13 +3483,13 @@
         <v>8</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>9</v>
@@ -3482,50 +3506,50 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B22" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E22" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="F22" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E23" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="F23" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="G23" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
@@ -3730,7 +3754,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
@@ -3741,7 +3765,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B55" t="s">
         <v>52</v>
@@ -3752,7 +3776,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B56" t="s">
         <v>52</v>
@@ -3761,62 +3785,110 @@
         <v>188</v>
       </c>
     </row>
-    <row customFormat="1" r="57" s="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="F57" s="24"/>
-    </row>
-    <row customFormat="1" r="58" s="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="F58" s="24"/>
-    </row>
-    <row customFormat="1" r="59" s="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="F59" s="24"/>
-    </row>
-    <row customFormat="1" r="60" s="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A60" s="21" t="s">
+    <row r="57">
+      <c r="A57" t="s">
+        <v>193</v>
+      </c>
+      <c r="B57" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>191</v>
+      </c>
+      <c r="B59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>189</v>
+      </c>
+      <c r="B61" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>187</v>
+      </c>
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row customFormat="1" r="63" s="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F63" s="24"/>
+    </row>
+    <row customFormat="1" r="64" s="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F64" s="24"/>
+    </row>
+    <row customFormat="1" r="65" s="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F65" s="24"/>
+    </row>
+    <row customFormat="1" r="66" s="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A66" s="21" t="s">
         <v>134</v>
       </c>
     </row>
-    <row customFormat="1" r="61" s="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A61" s="29" t="s">
+    <row customFormat="1" r="67" s="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A67" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row customFormat="1" r="62" s="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A62" s="30" t="s">
+    <row customFormat="1" r="68" s="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A68" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B68" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C68" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D62" s="30" t="s">
+      <c r="D68" s="30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row customFormat="1" r="63" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
-    <row customFormat="1" r="64" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
-    <row customFormat="1" r="65" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
-    <row customFormat="1" r="66" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
-    <row customFormat="1" r="67" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A68" s="27"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A69" s="27"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A70" s="27"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A71" s="27"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A72" s="27"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A73" s="27"/>
-    </row>
+    <row customFormat="1" r="69" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
+    <row customFormat="1" r="70" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
+    <row customFormat="1" r="71" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
+    <row customFormat="1" r="72" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
+    <row customFormat="1" r="73" s="14" spans="1:7" x14ac:dyDescent="0.15"/>
     <row r="74" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A74" s="27"/>
     </row>
@@ -4281,6 +4353,24 @@
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A228" s="27"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A229" s="27"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A230" s="27"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A231" s="27"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A232" s="27"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A233" s="27"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A234" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>